<commit_message>
Commiting Customer + Account files
</commit_message>
<xml_diff>
--- a/Data/CUSTOMERS.xlsx
+++ b/Data/CUSTOMERS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="67">
   <si>
     <t>TC</t>
   </si>
@@ -117,6 +117,102 @@
   </si>
   <si>
     <t>17704594</t>
+  </si>
+  <si>
+    <t>118500</t>
+  </si>
+  <si>
+    <t>17704735</t>
+  </si>
+  <si>
+    <t>6004</t>
+  </si>
+  <si>
+    <t>17704736</t>
+  </si>
+  <si>
+    <t>6020</t>
+  </si>
+  <si>
+    <t>118498</t>
+  </si>
+  <si>
+    <t>17704737</t>
+  </si>
+  <si>
+    <t>1001</t>
+  </si>
+  <si>
+    <t>17704738</t>
+  </si>
+  <si>
+    <t>17704739</t>
+  </si>
+  <si>
+    <t>6012</t>
+  </si>
+  <si>
+    <t>17704740</t>
+  </si>
+  <si>
+    <t>1047</t>
+  </si>
+  <si>
+    <t>17704741</t>
+  </si>
+  <si>
+    <t>1035</t>
+  </si>
+  <si>
+    <t>17704742</t>
+  </si>
+  <si>
+    <t>1150</t>
+  </si>
+  <si>
+    <t>17704743</t>
+  </si>
+  <si>
+    <t>1068</t>
+  </si>
+  <si>
+    <t>17704745</t>
+  </si>
+  <si>
+    <t>17704746</t>
+  </si>
+  <si>
+    <t>17704747</t>
+  </si>
+  <si>
+    <t>17704748</t>
+  </si>
+  <si>
+    <t>17704749</t>
+  </si>
+  <si>
+    <t>17704750</t>
+  </si>
+  <si>
+    <t>17704751</t>
+  </si>
+  <si>
+    <t>17704752</t>
+  </si>
+  <si>
+    <t>17704753</t>
+  </si>
+  <si>
+    <t>17704754</t>
+  </si>
+  <si>
+    <t>17704755</t>
+  </si>
+  <si>
+    <t>17704756</t>
+  </si>
+  <si>
+    <t>17704757</t>
   </si>
 </sst>
 </file>
@@ -161,7 +257,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -442,6 +538,248 @@
         <v>5</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Commiting Customer + Account files + ECRP
</commit_message>
<xml_diff>
--- a/Data/CUSTOMERS.xlsx
+++ b/Data/CUSTOMERS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="168">
   <si>
     <t>TC</t>
   </si>
@@ -351,6 +351,171 @@
   </si>
   <si>
     <t>17705020</t>
+  </si>
+  <si>
+    <t>17705034</t>
+  </si>
+  <si>
+    <t>17705035</t>
+  </si>
+  <si>
+    <t>1002</t>
+  </si>
+  <si>
+    <t>17705036</t>
+  </si>
+  <si>
+    <t>118464</t>
+  </si>
+  <si>
+    <t>17705037</t>
+  </si>
+  <si>
+    <t>1006</t>
+  </si>
+  <si>
+    <t>118465</t>
+  </si>
+  <si>
+    <t>17705038</t>
+  </si>
+  <si>
+    <t>1007</t>
+  </si>
+  <si>
+    <t>118466</t>
+  </si>
+  <si>
+    <t>17705039</t>
+  </si>
+  <si>
+    <t>118468</t>
+  </si>
+  <si>
+    <t>17705040</t>
+  </si>
+  <si>
+    <t>1177</t>
+  </si>
+  <si>
+    <t>118469</t>
+  </si>
+  <si>
+    <t>17705041</t>
+  </si>
+  <si>
+    <t>118470</t>
+  </si>
+  <si>
+    <t>17705042</t>
+  </si>
+  <si>
+    <t>6007</t>
+  </si>
+  <si>
+    <t>118471</t>
+  </si>
+  <si>
+    <t>17705043</t>
+  </si>
+  <si>
+    <t>1050</t>
+  </si>
+  <si>
+    <t>17705205</t>
+  </si>
+  <si>
+    <t>17705206</t>
+  </si>
+  <si>
+    <t>17705208</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>17705210</t>
+  </si>
+  <si>
+    <t>17705211</t>
+  </si>
+  <si>
+    <t>17705212</t>
+  </si>
+  <si>
+    <t>6005</t>
+  </si>
+  <si>
+    <t>17705214</t>
+  </si>
+  <si>
+    <t>1003</t>
+  </si>
+  <si>
+    <t>17705215</t>
+  </si>
+  <si>
+    <t>1033</t>
+  </si>
+  <si>
+    <t>17705224</t>
+  </si>
+  <si>
+    <t>17705225</t>
+  </si>
+  <si>
+    <t>17705226</t>
+  </si>
+  <si>
+    <t>17705229</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>17705230</t>
+  </si>
+  <si>
+    <t>17705231</t>
+  </si>
+  <si>
+    <t>17705232</t>
+  </si>
+  <si>
+    <t>17705233</t>
+  </si>
+  <si>
+    <t>17705234</t>
+  </si>
+  <si>
+    <t>17705235</t>
+  </si>
+  <si>
+    <t>17705238</t>
+  </si>
+  <si>
+    <t>17704245</t>
+  </si>
+  <si>
+    <t>17704413</t>
+  </si>
+  <si>
+    <t>17705259</t>
+  </si>
+  <si>
+    <t>17705260</t>
+  </si>
+  <si>
+    <t>17705261</t>
+  </si>
+  <si>
+    <t>17705262</t>
+  </si>
+  <si>
+    <t>17705263</t>
+  </si>
+  <si>
+    <t>1011</t>
   </si>
 </sst>
 </file>
@@ -395,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1402,6 +1567,402 @@
         <v>42</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" t="s">
+        <v>113</v>
+      </c>
+      <c r="C92" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" t="s">
+        <v>114</v>
+      </c>
+      <c r="C93" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>106</v>
+      </c>
+      <c r="B94" t="s">
+        <v>116</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>117</v>
+      </c>
+      <c r="B95" t="s">
+        <v>118</v>
+      </c>
+      <c r="C95" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>120</v>
+      </c>
+      <c r="B96" t="s">
+        <v>121</v>
+      </c>
+      <c r="C96" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>123</v>
+      </c>
+      <c r="B97" t="s">
+        <v>124</v>
+      </c>
+      <c r="C97" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>125</v>
+      </c>
+      <c r="B98" t="s">
+        <v>126</v>
+      </c>
+      <c r="C98" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>128</v>
+      </c>
+      <c r="B99" t="s">
+        <v>129</v>
+      </c>
+      <c r="C99" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>130</v>
+      </c>
+      <c r="B100" t="s">
+        <v>131</v>
+      </c>
+      <c r="C100" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>133</v>
+      </c>
+      <c r="B101" t="s">
+        <v>134</v>
+      </c>
+      <c r="C101" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>106</v>
+      </c>
+      <c r="B102" t="s">
+        <v>136</v>
+      </c>
+      <c r="C102" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>106</v>
+      </c>
+      <c r="B103" t="s">
+        <v>137</v>
+      </c>
+      <c r="C103" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>117</v>
+      </c>
+      <c r="B104" t="s">
+        <v>138</v>
+      </c>
+      <c r="C104" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>123</v>
+      </c>
+      <c r="B105" t="s">
+        <v>140</v>
+      </c>
+      <c r="C105" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>125</v>
+      </c>
+      <c r="B106" t="s">
+        <v>141</v>
+      </c>
+      <c r="C106" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>128</v>
+      </c>
+      <c r="B107" t="s">
+        <v>142</v>
+      </c>
+      <c r="C107" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>130</v>
+      </c>
+      <c r="B108" t="s">
+        <v>144</v>
+      </c>
+      <c r="C108" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>133</v>
+      </c>
+      <c r="B109" t="s">
+        <v>146</v>
+      </c>
+      <c r="C109" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>106</v>
+      </c>
+      <c r="B110" t="s">
+        <v>148</v>
+      </c>
+      <c r="C110" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" t="s">
+        <v>149</v>
+      </c>
+      <c r="C111" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>106</v>
+      </c>
+      <c r="B112" t="s">
+        <v>150</v>
+      </c>
+      <c r="C112" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>106</v>
+      </c>
+      <c r="B113" t="s">
+        <v>151</v>
+      </c>
+      <c r="C113" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>106</v>
+      </c>
+      <c r="B114" t="s">
+        <v>153</v>
+      </c>
+      <c r="C114" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>106</v>
+      </c>
+      <c r="B115" t="s">
+        <v>154</v>
+      </c>
+      <c r="C115" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>117</v>
+      </c>
+      <c r="B116" t="s">
+        <v>155</v>
+      </c>
+      <c r="C116" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>120</v>
+      </c>
+      <c r="B117" t="s">
+        <v>156</v>
+      </c>
+      <c r="C117" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>123</v>
+      </c>
+      <c r="B118" t="s">
+        <v>157</v>
+      </c>
+      <c r="C118" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>125</v>
+      </c>
+      <c r="B119" t="s">
+        <v>158</v>
+      </c>
+      <c r="C119" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>133</v>
+      </c>
+      <c r="B120" t="s">
+        <v>159</v>
+      </c>
+      <c r="C120" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>152</v>
+      </c>
+      <c r="B121" t="s">
+        <v>160</v>
+      </c>
+      <c r="C121" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>152</v>
+      </c>
+      <c r="B122" t="s">
+        <v>161</v>
+      </c>
+      <c r="C122" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>106</v>
+      </c>
+      <c r="B123" t="s">
+        <v>162</v>
+      </c>
+      <c r="C123" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>106</v>
+      </c>
+      <c r="B124" t="s">
+        <v>163</v>
+      </c>
+      <c r="C124" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>106</v>
+      </c>
+      <c r="B125" t="s">
+        <v>164</v>
+      </c>
+      <c r="C125" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>117</v>
+      </c>
+      <c r="B126" t="s">
+        <v>165</v>
+      </c>
+      <c r="C126" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>120</v>
+      </c>
+      <c r="B127" t="s">
+        <v>166</v>
+      </c>
+      <c r="C127" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Commiting different scripts + their data
</commit_message>
<xml_diff>
--- a/Data/CUSTOMERS.xlsx
+++ b/Data/CUSTOMERS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="183">
   <si>
     <t>TC</t>
   </si>
@@ -516,6 +516,51 @@
   </si>
   <si>
     <t>1011</t>
+  </si>
+  <si>
+    <t>17706585</t>
+  </si>
+  <si>
+    <t>17706586</t>
+  </si>
+  <si>
+    <t>17706587</t>
+  </si>
+  <si>
+    <t>17706588</t>
+  </si>
+  <si>
+    <t>17706589</t>
+  </si>
+  <si>
+    <t>17706590</t>
+  </si>
+  <si>
+    <t>17706591</t>
+  </si>
+  <si>
+    <t>17706592</t>
+  </si>
+  <si>
+    <t>17707507</t>
+  </si>
+  <si>
+    <t>17707512</t>
+  </si>
+  <si>
+    <t>17707515</t>
+  </si>
+  <si>
+    <t>17707516</t>
+  </si>
+  <si>
+    <t>17707517</t>
+  </si>
+  <si>
+    <t>17707519</t>
+  </si>
+  <si>
+    <t>17707520</t>
   </si>
 </sst>
 </file>
@@ -560,7 +605,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1963,6 +2008,171 @@
         <v>167</v>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>35</v>
+      </c>
+      <c r="B128" t="s">
+        <v>168</v>
+      </c>
+      <c r="C128" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" t="s">
+        <v>169</v>
+      </c>
+      <c r="C129" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>40</v>
+      </c>
+      <c r="B130" t="s">
+        <v>170</v>
+      </c>
+      <c r="C130" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131" t="s">
+        <v>171</v>
+      </c>
+      <c r="C131" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" t="s">
+        <v>172</v>
+      </c>
+      <c r="C132" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>13</v>
+      </c>
+      <c r="B133" t="s">
+        <v>173</v>
+      </c>
+      <c r="C133" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>7</v>
+      </c>
+      <c r="B134" t="s">
+        <v>174</v>
+      </c>
+      <c r="C134" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>3</v>
+      </c>
+      <c r="B135" t="s">
+        <v>175</v>
+      </c>
+      <c r="C135" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>106</v>
+      </c>
+      <c r="B136" t="s">
+        <v>176</v>
+      </c>
+      <c r="C136" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>106</v>
+      </c>
+      <c r="B137" t="s">
+        <v>177</v>
+      </c>
+      <c r="C137" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>106</v>
+      </c>
+      <c r="B138" t="s">
+        <v>178</v>
+      </c>
+      <c r="C138" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>106</v>
+      </c>
+      <c r="B139" t="s">
+        <v>179</v>
+      </c>
+      <c r="C139" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>106</v>
+      </c>
+      <c r="B140" t="s">
+        <v>180</v>
+      </c>
+      <c r="C140" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>117</v>
+      </c>
+      <c r="B141" t="s">
+        <v>181</v>
+      </c>
+      <c r="C141" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>120</v>
+      </c>
+      <c r="B142" t="s">
+        <v>182</v>
+      </c>
+      <c r="C142" t="s">
+        <v>167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>